<commit_message>
updated RTM (separate CM and SIQ columns)
updated RTM (separate CM and SIQ columns) according to review
</commit_message>
<xml_diff>
--- a/Project Management/Travel_RTM.xlsx
+++ b/Project Management/Travel_RTM.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="48">
   <si>
     <t>RTM</t>
   </si>
@@ -147,6 +147,15 @@
   </si>
   <si>
     <t>SRS_Rtng_Fbk_3</t>
+  </si>
+  <si>
+    <t>Const_3</t>
+  </si>
+  <si>
+    <t>Admn_feat_1</t>
+  </si>
+  <si>
+    <t>SRS_Admn_1</t>
   </si>
 </sst>
 </file>
@@ -1244,9 +1253,15 @@
       <c r="R25" s="26"/>
     </row>
     <row r="26">
-      <c r="B26" s="34"/>
-      <c r="C26" s="34"/>
-      <c r="D26" s="34"/>
+      <c r="B26" s="23" t="s">
+        <v>45</v>
+      </c>
+      <c r="C26" s="23" t="s">
+        <v>46</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>47</v>
+      </c>
       <c r="E26" s="24"/>
       <c r="F26" s="25"/>
       <c r="G26" s="9"/>

</xml_diff>